<commit_message>
fix university of derby inconsistency
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="619">
   <si>
     <t>BRAWL</t>
   </si>
@@ -1861,21 +1861,12 @@
     <t>Kiah Greenwood</t>
   </si>
   <si>
-    <t>university</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
     <t>VAGUE Vets</t>
   </si>
   <si>
     <t>Vanguard VETS</t>
   </si>
   <si>
-    <t>uni of darby</t>
-  </si>
-  <si>
     <t>GEAS wargamers</t>
   </si>
   <si>
@@ -1886,6 +1877,12 @@
   </si>
   <si>
     <t>Fantasy (open classic)</t>
+  </si>
+  <si>
+    <t>university_name</t>
+  </si>
+  <si>
+    <t>category_name</t>
   </si>
 </sst>
 </file>
@@ -2205,8 +2202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2261,7 +2258,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -2331,12 +2328,12 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -2361,7 +2358,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>615</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -2381,12 +2378,12 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -2427,8 +2424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C531"/>
   <sheetViews>
-    <sheetView topLeftCell="A460" workbookViewId="0">
-      <selection activeCell="C472" sqref="C472"/>
+    <sheetView topLeftCell="A355" workbookViewId="0">
+      <selection activeCell="B374" sqref="B374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,10 +2440,10 @@
         <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="C1" t="s">
-        <v>612</v>
+        <v>618</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3546,7 +3543,7 @@
         <v>47</v>
       </c>
       <c r="C101" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3557,7 +3554,7 @@
         <v>73</v>
       </c>
       <c r="C102" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -3568,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="C103" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -3579,7 +3576,7 @@
         <v>77</v>
       </c>
       <c r="C104" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -3590,7 +3587,7 @@
         <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3601,7 +3598,7 @@
         <v>164</v>
       </c>
       <c r="C106" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3612,7 +3609,7 @@
         <v>47</v>
       </c>
       <c r="C107" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -3623,7 +3620,7 @@
         <v>77</v>
       </c>
       <c r="C108" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3634,7 +3631,7 @@
         <v>51</v>
       </c>
       <c r="C109" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -3645,7 +3642,7 @@
         <v>79</v>
       </c>
       <c r="C110" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3656,7 +3653,7 @@
         <v>51</v>
       </c>
       <c r="C111" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3667,7 +3664,7 @@
         <v>65</v>
       </c>
       <c r="C112" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3678,7 +3675,7 @@
         <v>119</v>
       </c>
       <c r="C113" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3689,7 +3686,7 @@
         <v>79</v>
       </c>
       <c r="C114" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3700,7 +3697,7 @@
         <v>7</v>
       </c>
       <c r="C115" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -5820,7 +5817,7 @@
         <v>359</v>
       </c>
       <c r="B308" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C308" t="s">
         <v>32</v>
@@ -6447,7 +6444,7 @@
         <v>411</v>
       </c>
       <c r="B365" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C365" t="s">
         <v>37</v>
@@ -7877,7 +7874,7 @@
         <v>544</v>
       </c>
       <c r="B495" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C495" t="s">
         <v>579</v>
@@ -8152,7 +8149,7 @@
         <v>569</v>
       </c>
       <c r="B520" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C520" t="s">
         <v>43</v>
@@ -8289,8 +8286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8345,7 +8342,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>